<commit_message>
modified:   code.ipynb 	deleted:    "results/\350\200\225\345\234\260\351\235\242\347\247\257\345\210\206\345\270\203\351\245\274\345\233\276.png" 	new file:   "results/\350\200\225\345\234\260\351\235\242\347\247\257\345\210\206\345\270\203\351\245\274\345\233\276_\345\244\247\346\243\232.png" 	new file:   "results/\350\200\225\345\234\260\351\235\242\347\247\257\345\210\206\345\270\203\351\245\274\345\233\276_\346\227\240\345\244\247\346\243\232.png" 	new file:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/~$\351\231\204\344\273\2661.xlsx" 	new file:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/~$\351\231\204\344\273\2662.xlsx" 	modified:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/\351\231\204\344\273\2661.xlsx"
</commit_message>
<xml_diff>
--- a/题目及附件/附件1.xlsx
+++ b/题目及附件/附件1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Math_model\CUMCM2024Problems\C题\题目及附件\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516C3858-6F29-49E3-B4F2-A47C166C264C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59BE13D-FA58-4A70-BF03-2C7D19D332E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="3320" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="乡村的现有耕地" sheetId="10" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="119">
   <si>
     <t>A1</t>
   </si>
@@ -677,42 +677,286 @@
     <r>
       <rPr>
         <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>刀豆</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>芸豆</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>土豆</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>水浇地</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
+      <t>蔬菜</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>西红柿</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>茄子</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>菠菜</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第一季
-普通大棚</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>青椒</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>菜花</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>包菜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>油麦菜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>小青菜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>黄瓜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>生菜</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>辣椒</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>空心菜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>黄心菜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>芹菜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>大白菜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>白萝卜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红萝卜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>榆黄菇</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -721,388 +965,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>第一季
-智慧大棚</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">第一季、第二季
-</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>刀豆</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>芸豆</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>土豆</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>蔬菜</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>西红柿</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>茄子</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>菠菜</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>青椒</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>菜花</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>包菜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>油麦菜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>小青菜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>黄瓜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>生菜</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>辣椒</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>空心菜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>黄心菜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>芹菜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>大白菜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>水浇地</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第二季</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>白萝卜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>红萝卜</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>榆黄菇</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
       <t>食用菌</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>普通大棚</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第二季</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1147,6 +1010,67 @@
 梯田
 山坡地
 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通大棚第二季</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>水浇地第二季</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>水浇地第一季</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>普通大棚第一季</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>智慧大棚第一季、第二季</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1154,7 +1078,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1235,6 +1159,20 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1294,7 +1232,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1340,14 +1278,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2292,8 +2227,8 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2301,7 +2236,7 @@
     <col min="1" max="1" width="9.08984375" style="6" customWidth="1"/>
     <col min="2" max="2" width="11.36328125" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.453125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" style="4" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
@@ -2319,7 +2254,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="54.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2329,11 +2264,11 @@
       <c r="C2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D2" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2343,9 +2278,11 @@
       <c r="C3" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D3" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2355,9 +2292,11 @@
       <c r="C4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D4" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2367,9 +2306,11 @@
       <c r="C5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D5" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2379,9 +2320,11 @@
       <c r="C6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2391,9 +2334,11 @@
       <c r="C7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2403,9 +2348,11 @@
       <c r="C8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2415,9 +2362,11 @@
       <c r="C9" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2427,9 +2376,11 @@
       <c r="C10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D10" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2439,9 +2390,11 @@
       <c r="C11" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D11" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2451,9 +2404,11 @@
       <c r="C12" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D12" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2463,9 +2418,11 @@
       <c r="C13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D13" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2475,9 +2432,11 @@
       <c r="C14" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D14" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2487,9 +2446,11 @@
       <c r="C15" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D15" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2499,7 +2460,9 @@
       <c r="C16" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -2515,7 +2478,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2525,226 +2488,260 @@
       <c r="C18" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D18" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="16"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D19" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="16"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D20" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="16"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D21" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="16"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="16"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="16"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="16"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="16"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="16"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="16"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="16"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="16"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="16"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="16"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
@@ -2752,37 +2749,41 @@
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="15"/>
+        <v>92</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="15"/>
+        <v>92</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
@@ -2790,36 +2791,42 @@
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D40" s="15"/>
+        <v>111</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="15"/>
     </row>
     <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="15"/>
+        <v>111</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
@@ -2846,12 +2853,6 @@
       <c r="D46" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D2:D16"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="D18:D35"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>